<commit_message>
CIDC-1069 add reports file
</commit_message>
<xml_diff>
--- a/template_examples/atacseq_analysis_template.xlsx
+++ b/template_examples/atacseq_analysis_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/VSCodeProjects/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95C78118-C4F0-0042-BAEB-E1E027B9DE74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE68EC9-B195-9447-B84A-430D111B38E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="16380" windowHeight="8200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -196,10 +196,10 @@
     <t>A comment describing why this sample is missing from the pipeline output.</t>
   </si>
   <si>
-    <t>Report</t>
+    <t>Reports</t>
   </si>
   <si>
-    <t>report/report.zip</t>
+    <t>test_prism_trial_id/atacseq/analysis/reports.zip</t>
   </si>
 </sst>
 </file>
@@ -713,7 +713,7 @@
   <dimension ref="A1:C2007"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -753,7 +753,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="33" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
CIDC-1069 move atacseq to components/ngs
</commit_message>
<xml_diff>
--- a/template_examples/atacseq_analysis_template.xlsx
+++ b/template_examples/atacseq_analysis_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/VSCodeProjects/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9EF39CC-C334-C349-87B8-002EB471947A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E16E77A3-0C6A-694A-AEFC-4594DF048862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="16380" windowHeight="8200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -199,13 +199,13 @@
     <t>Report</t>
   </si>
   <si>
-    <t>test_prism_trial_id/atacseq/analysis/report.zip</t>
-  </si>
-  <si>
     <t>Batch id</t>
   </si>
   <si>
     <t>XYZ</t>
+  </si>
+  <si>
+    <t>test_prism_trial_id/atacseq/analysis/XYZ/report.zip</t>
   </si>
 </sst>
 </file>
@@ -719,7 +719,7 @@
   <dimension ref="A1:C2008"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -764,10 +764,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="33" thickBot="1" x14ac:dyDescent="0.25">
@@ -778,7 +778,7 @@
         <v>30</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
CIDC-1278 first pass at redone docs
</commit_message>
<xml_diff>
--- a/template_examples/atacseq_analysis_template.xlsx
+++ b/template_examples/atacseq_analysis_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="ATACSEQ Analysis" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="ATACseq Analysis" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Excluded Samples" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Legend" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Data Dictionary" sheetId="4" state="visible" r:id="rId5"/>
@@ -180,7 +180,7 @@
     <t xml:space="preserve">#skip</t>
   </si>
   <si>
-    <t xml:space="preserve">ATACSEQ Runs</t>
+    <t xml:space="preserve">ATACSeq Runs</t>
   </si>
   <si>
     <t xml:space="preserve">#header</t>
@@ -219,7 +219,7 @@
     <t xml:space="preserve">LEGEND</t>
   </si>
   <si>
-    <t xml:space="preserve">Legend for tab 'ATACSEQ Analysis'</t>
+    <t xml:space="preserve">Legend for tab 'ATACSeq Analysis'</t>
   </si>
   <si>
     <t xml:space="preserve">String</t>
@@ -234,7 +234,7 @@
     <t xml:space="preserve">Path to a file on a user's computer.</t>
   </si>
   <si>
-    <t xml:space="preserve">Section 'ATACSEQ Runs' of tab 'ATACSEQ Analysis'</t>
+    <t xml:space="preserve">Section 'ATACSeq Runs' of tab 'ATACSeq Analysis'</t>
   </si>
   <si>
     <t xml:space="preserve">String: regex ^C[A-Z0-9]{3}[A-Z0-9]{3}[A-Z0-9]{2}.[0-9]{2}$ </t>
@@ -502,10 +502,10 @@
   <dimension ref="A1:C2008"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="1" sqref="B3:C4 B9"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.2890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.30859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="1" style="0" width="30.7"/>
   </cols>
@@ -10612,11 +10612,11 @@
   </sheetPr>
   <dimension ref="A1:C2002"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3:C4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.2890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.30859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="1" style="0" width="30.7"/>
   </cols>
@@ -20675,11 +20675,11 @@
   </sheetPr>
   <dimension ref="B1:E13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B3:C4 A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.2890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.30859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="2" style="0" width="30.7"/>
   </cols>
@@ -20689,7 +20689,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
         <v>25</v>
       </c>
@@ -20735,7 +20735,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1" t="s">
         <v>30</v>
       </c>
@@ -20820,10 +20820,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B3:C4 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.2890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.30859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="2" style="0" width="30.7"/>
   </cols>

</xml_diff>

<commit_message>
CIDC-1526 filepath docs, manifest tweaks
</commit_message>
<xml_diff>
--- a/template_examples/atacseq_analysis_template.xlsx
+++ b/template_examples/atacseq_analysis_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ATACseq Analysis" sheetId="1" state="visible" r:id="rId2"/>
@@ -66,7 +66,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Path to a file on a user's computer.
+          <t xml:space="preserve">Path to file, relative to the intake bucket.
 In .zip format</t>
         </r>
       </text>
@@ -81,7 +81,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Specimen identifier assigned by the CIMAC-CIDC Network. Formatted as C????????.??</t>
+          <t xml:space="preserve">Specimen identifier assigned by the CIMAC-CIDC Network. Formatted as CTTTPPPSS.AA for trial code TTT, participant PPP, sample SS, and aliquot AA.</t>
         </r>
       </text>
     </comment>
@@ -119,7 +119,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">Specimen identifier assigned by the CIMAC-CIDC Network. Formatted as C????????.??</t>
+          <t xml:space="preserve">Specimen identifier assigned by the CIMAC-CIDC Network. Formatted as CTTTPPPSS.AA for trial code TTT, participant PPP, sample SS, and aliquot AA.</t>
         </r>
       </text>
     </comment>
@@ -180,7 +180,7 @@
     <t xml:space="preserve">#skip</t>
   </si>
   <si>
-    <t xml:space="preserve">ATACSeq Runs</t>
+    <t xml:space="preserve">ATACseq Runs</t>
   </si>
   <si>
     <t xml:space="preserve">#header</t>
@@ -219,7 +219,7 @@
     <t xml:space="preserve">LEGEND</t>
   </si>
   <si>
-    <t xml:space="preserve">Legend for tab 'ATACSeq Analysis'</t>
+    <t xml:space="preserve">Legend for tab 'ATACseq Analysis'</t>
   </si>
   <si>
     <t xml:space="preserve">String</t>
@@ -231,16 +231,16 @@
     <t xml:space="preserve">ATACseq batch identification number. Unique to every batch.</t>
   </si>
   <si>
-    <t xml:space="preserve">Path to a file on a user's computer.</t>
+    <t xml:space="preserve">Path to file, relative to the intake bucket.</t>
   </si>
   <si>
-    <t xml:space="preserve">Section 'ATACSeq Runs' of tab 'ATACSeq Analysis'</t>
+    <t xml:space="preserve">Section 'ATACseq Runs' of tab 'ATACseq Analysis'</t>
   </si>
   <si>
     <t xml:space="preserve">String: regex ^C[A-Z0-9]{3}[A-Z0-9]{3}[A-Z0-9]{2}.[0-9]{2}$ </t>
   </si>
   <si>
-    <t xml:space="preserve">Specimen identifier assigned by the CIMAC-CIDC Network. Formatted as C????????.??</t>
+    <t xml:space="preserve">Specimen identifier assigned by the CIMAC-CIDC Network. Formatted as CTTTPPPSS.AA for trial code TTT, participant PPP, sample SS, and aliquot AA.</t>
   </si>
   <si>
     <t xml:space="preserve">E.g. 'CTTTP01A1.00'</t>
@@ -501,11 +501,11 @@
   </sheetPr>
   <dimension ref="A1:C2008"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B9" activeCellId="1" sqref="B3:C4 B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.30859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.28125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="1" style="0" width="30.7"/>
   </cols>
@@ -10612,11 +10612,11 @@
   </sheetPr>
   <dimension ref="A1:C2002"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.30859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.28125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="1" style="0" width="30.7"/>
   </cols>
@@ -20675,11 +20675,11 @@
   </sheetPr>
   <dimension ref="B1:E13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B3:C4 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.30859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.28125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="2" style="0" width="30.7"/>
   </cols>
@@ -20689,7 +20689,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
         <v>25</v>
       </c>
@@ -20735,7 +20735,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1" t="s">
         <v>30</v>
       </c>
@@ -20820,10 +20820,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B3:C4 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.30859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.28125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="2" style="0" width="30.7"/>
   </cols>

</xml_diff>